<commit_message>
Punctaj lab 1 grupa 3
</commit_message>
<xml_diff>
--- a/2019/30133.xlsx
+++ b/2019/30133.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\dt\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7EC255-EFF8-4492-973B-7A6A1B8B853B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C8E71B-9277-4CF0-BD9E-4AA32A43F49F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5D8816DA-82BD-435A-B96D-1E869846659E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="40">
   <si>
     <t>Alecusan Raluca - Sonia</t>
   </si>
@@ -142,6 +142,15 @@
   </si>
   <si>
     <t>PUNCTAJ</t>
+  </si>
+  <si>
+    <t>8,5</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>Leahu Stefanel</t>
   </si>
 </sst>
 </file>
@@ -207,7 +216,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -285,33 +294,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.34998626667073579"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD3D3D3"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFD3D3D3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD3D3D3"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -636,8 +738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64FC518A-FA3D-453E-BD9E-77B969FB8DBB}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -646,339 +748,538 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A2" s="6">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="2"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="9"/>
-      <c r="D3" s="1"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A4" s="6">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="9"/>
-      <c r="D4" s="1"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A5" s="6">
+      <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="9"/>
-      <c r="D5" s="1"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A6" s="6">
+      <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A7" s="6">
+      <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="9"/>
-      <c r="D7" s="1"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A8" s="6">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="9"/>
-      <c r="D8" s="1"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A9" s="6">
+      <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="9"/>
-      <c r="D9" s="1"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A10" s="6">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="1"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A11" s="6">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="9"/>
-      <c r="D11" s="1"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A12" s="6">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="1"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A13" s="6">
+      <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="9"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A14" s="6">
+      <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="9"/>
-      <c r="D14" s="1"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A15" s="6">
+      <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="9"/>
-      <c r="D15" s="1"/>
-      <c r="G15" s="4"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" ht="14.4" customHeight="1">
-      <c r="A16" s="6">
+      <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="9"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A17" s="6">
+      <c r="D16" s="10"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="9"/>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A18" s="6">
+      <c r="D17" s="10"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A19" s="6">
+      <c r="D18" s="10"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C19" s="9"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A20" s="6">
+      <c r="D19" s="10"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A21" s="6">
+      <c r="C20" s="9">
+        <v>9</v>
+      </c>
+      <c r="D20" s="10"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="9"/>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A22" s="6">
+      <c r="C21" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="10"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="9"/>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A23" s="6">
+      <c r="C22" s="9">
+        <v>4</v>
+      </c>
+      <c r="D22" s="10"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="9"/>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A24" s="6">
+      <c r="C23" s="9">
+        <v>5</v>
+      </c>
+      <c r="D23" s="10"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A24" s="3">
         <v>23</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A25" s="6">
+      <c r="C24" s="9">
+        <v>7</v>
+      </c>
+      <c r="D24" s="10"/>
+      <c r="E24" s="8"/>
+      <c r="F24" s="8"/>
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A25" s="3">
         <v>24</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A26" s="6">
+      <c r="C25" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" s="10"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A26" s="3">
         <v>25</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A27" s="6">
+      <c r="C26" s="9">
+        <v>9</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A27" s="3">
         <v>26</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="9"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A28" s="6">
+      <c r="D27" s="10"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A28" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="9"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A29" s="6">
+      <c r="D28" s="10"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A29" s="3">
         <v>28</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" ht="14.4" customHeight="1">
-      <c r="A30" s="6">
+      <c r="C29" s="9">
+        <v>6</v>
+      </c>
+      <c r="D29" s="10"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" ht="14.4" customHeight="1">
+      <c r="A30" s="15">
         <v>29</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="9"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:8">
-      <c r="A31" s="5"/>
-    </row>
-    <row r="32" spans="1:8">
-      <c r="A32" s="5"/>
-      <c r="H32" s="5"/>
+      <c r="C30" s="18">
+        <v>7</v>
+      </c>
+      <c r="D30" s="17"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="14">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32" s="2"/>
+      <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="5"/>
+      <c r="A33" s="2"/>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="5"/>
+      <c r="A34" s="2"/>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="5"/>
+      <c r="A35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>